<commit_message>
Update with latest BNEF battery pack prices
</commit_message>
<xml_diff>
--- a/InputData/trans/BPP/Battery Pack Price.xlsx
+++ b/InputData/trans/BPP/Battery Pack Price.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\BPP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6A0AE7-8BAD-4DD4-8CEE-F481B181AB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48359E06-F382-4E1F-81F2-5E8970E7301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{DC12087C-9A27-4A43-B4A9-6B3F1E517F08}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Sources:</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>The EPS applies endogenous learning for battery pack prices in years where the battery pack price is listed as 0.</t>
+  </si>
+  <si>
+    <t>2022 to 2023</t>
+  </si>
+  <si>
+    <t>Lithium-ion Battery Pack Prices Hit Record Low of $139/kWh</t>
+  </si>
+  <si>
+    <t>https://about.bnef.com/blog/lithium-ion-battery-pack-prices-hit-record-low-of-139-kwh/#:~:text=Given%20this%2C%20BNEF%20expects%20average,and%20%2480%2FkWh%20in%202030.</t>
   </si>
 </sst>
 </file>
@@ -428,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF982137-6F01-4109-8226-D4C6F3731BA9}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,21 +477,50 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>1.29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>1/0.951</f>
+        <v>1.0515247108307046</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -498,7 +536,7 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,15 +641,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <f>141/About!$A$11</f>
+        <f>141/About!$A$16</f>
         <v>109.30232558139535</v>
       </c>
       <c r="C2">
-        <f>151/About!$A$11</f>
+        <f>151/About!$A$16</f>
         <v>117.05426356589147</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <f>139/(About!A16*About!A17)</f>
+        <v>102.47209302325579</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -726,7 +765,7 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <f>150/About!$A$11</f>
+        <f>150/About!$A$16</f>
         <v>116.27906976744185</v>
       </c>
     </row>

</xml_diff>